<commit_message>
minor adjustment of the description in perf section
git-svn-id: file://localhost/tmp/svn2git/svn@7189 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/sc/pilot-data-exp.xlsx
+++ b/papers/troy/pstar/perf/sc/pilot-data-exp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="50380" windowHeight="28360" tabRatio="500" activeTab="6"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="50380" windowHeight="28360" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Trestles" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <pivotCache cacheId="1" r:id="rId9"/>
     <pivotCache cacheId="2" r:id="rId10"/>
     <pivotCache cacheId="3" r:id="rId11"/>
-    <pivotCache cacheId="8" r:id="rId12"/>
+    <pivotCache cacheId="11" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1163,9 +1163,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Total!$A$4:$A$7</c:f>
+              <c:f>Total!$A$4:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>No PD_x000d_(Trestles)</c:v>
                 </c:pt>
@@ -1175,18 +1175,15 @@
                 <c:pt idx="2">
                   <c:v>PD/Globus Online_x000d_(Trestles)</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>DIANE/SRM_x000d_(EGI)</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Total!$B$4:$B$7</c:f>
+              <c:f>Total!$B$4:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0" formatCode="0">
                   <c:v>178.7429249762583</c:v>
                 </c:pt>
@@ -1195,9 +1192,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>34.36352397203778</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.196921158333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1242,7 +1236,7 @@
                     <c:v>5.095156348019516</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>21.88203898764747</c:v>
+                    <c:v>9.021936580237572</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>3.079859904444445</c:v>
@@ -1263,7 +1257,7 @@
                     <c:v>5.095156348019516</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>21.88203898764747</c:v>
+                    <c:v>9.021936580237572</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>3.079859904444445</c:v>
@@ -1274,9 +1268,9 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Total!$A$4:$A$7</c:f>
+              <c:f>Total!$A$4:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>No PD_x000d_(Trestles)</c:v>
                 </c:pt>
@@ -1286,18 +1280,15 @@
                 <c:pt idx="2">
                   <c:v>PD/Globus Online_x000d_(Trestles)</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>DIANE/SRM_x000d_(EGI)</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Total!$D$4:$D$7</c:f>
+              <c:f>Total!$D$4:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>39.22208226540834</c:v>
                 </c:pt>
@@ -1305,10 +1296,7 @@
                   <c:v>20.47924295277776</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.24849434027777</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15.59591256055555</c:v>
+                  <c:v>12.83431719538888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1691,7 +1679,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41031.785144328707" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="3">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41031.875360532409" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="3">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:O4" sheet="BJ (PD-GO)"/>
   </cacheSource>
@@ -1735,13 +1723,13 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="13.8371118531" maxValue="16.926529794899999"/>
     </cacheField>
     <cacheField name="Net Runtime" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="835.58040403999985" maxValue="2954.5518860799993"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="835.58040403999985" maxValue="1474.5966911300002"/>
     </cacheField>
     <cacheField name="Staging" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1922.4414711048" maxValue="2331.2698736151997"/>
     </cacheField>
     <cacheField name="Runtime + Staging" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2758.0218751448001" maxValue="5285.821759695199"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2331.2698736151997" maxValue="3406.3196613768005"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -5860,9 +5848,9 @@
     <s v="pbs-ssh://luckow@trestles.sdsc.edu"/>
     <n v="164.674059868"/>
     <n v="16.926529794899999"/>
-    <n v="2954.5518860799993"/>
+    <m/>
     <n v="2331.2698736151997"/>
-    <n v="5285.821759695199"/>
+    <n v="2331.2698736151997"/>
   </r>
   <r>
     <n v="1"/>
@@ -6163,7 +6151,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="Q5:U8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField showAll="0"/>
@@ -19268,7 +19256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2:U6"/>
       <pivotSelection pane="bottomRight" showHeader="1" activeRow="1" activeCol="16" click="1" r:id="rId1">
         <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
@@ -19872,8 +19860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -19980,17 +19968,13 @@
       <c r="L2">
         <v>16.926529794899999</v>
       </c>
-      <c r="M2">
-        <f t="shared" ref="M2:M4" si="0">G2-F2</f>
-        <v>2954.5518860799993</v>
-      </c>
       <c r="N2">
-        <f t="shared" ref="N2:N4" si="1">K2+L2*E2</f>
+        <f t="shared" ref="N2:N4" si="0">K2+L2*E2</f>
         <v>2331.2698736151997</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O4" si="2">N2+M2</f>
-        <v>5285.821759695199</v>
+        <f t="shared" ref="O2:O4" si="1">N2+M2</f>
+        <v>2331.2698736151997</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -20031,15 +20015,15 @@
         <v>13.8936581891</v>
       </c>
       <c r="M3">
+        <f t="shared" ref="M2:M4" si="2">G3-F3</f>
+        <v>1474.5966911300002</v>
+      </c>
+      <c r="N3">
         <f t="shared" si="0"/>
-        <v>1474.5966911300002</v>
-      </c>
-      <c r="N3">
+        <v>1931.7229702468001</v>
+      </c>
+      <c r="O3">
         <f t="shared" si="1"/>
-        <v>1931.7229702468001</v>
-      </c>
-      <c r="O3">
-        <f t="shared" si="2"/>
         <v>3406.3196613768005</v>
       </c>
     </row>
@@ -20081,15 +20065,15 @@
         <v>13.8371118531</v>
       </c>
       <c r="M4">
+        <f t="shared" si="2"/>
+        <v>835.58040403999985</v>
+      </c>
+      <c r="N4">
         <f t="shared" si="0"/>
-        <v>835.58040403999985</v>
-      </c>
-      <c r="N4">
+        <v>1922.4414711048</v>
+      </c>
+      <c r="O4">
         <f t="shared" si="1"/>
-        <v>1922.4414711048</v>
-      </c>
-      <c r="O4">
-        <f t="shared" si="2"/>
         <v>2758.0218751448001</v>
       </c>
     </row>
@@ -20123,13 +20107,13 @@
         <v>2061.8114383222669</v>
       </c>
       <c r="S7" s="8">
-        <v>3816.7210987389335</v>
+        <v>2831.8704700456001</v>
       </c>
       <c r="T7" s="8">
         <v>233.40399058171062</v>
       </c>
       <c r="U7" s="8">
-        <v>1312.9223392588483</v>
+        <v>541.31619481425435</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -20140,13 +20124,13 @@
         <v>2061.8114383222669</v>
       </c>
       <c r="S8" s="5">
-        <v>3816.7210987389335</v>
+        <v>2831.8704700456001</v>
       </c>
       <c r="T8" s="5">
         <v>233.40399058171062</v>
       </c>
       <c r="U8" s="5">
-        <v>1312.9223392588483</v>
+        <v>541.31619481425435</v>
       </c>
     </row>
   </sheetData>
@@ -20259,8 +20243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20340,15 +20324,15 @@
       </c>
       <c r="C6" s="8">
         <f>'BJ (PD-GO)'!S7/60</f>
-        <v>63.612018312315556</v>
+        <v>47.197841167426667</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="0"/>
-        <v>29.248494340277773</v>
+        <v>12.834317195388884</v>
       </c>
       <c r="E6" s="8">
         <f>'BJ (PD-GO)'!U7/60</f>
-        <v>21.882038987647473</v>
+        <v>9.0219365802375719</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">

</xml_diff>